<commit_message>
Added test cases from BANK_SYS_TC_TR_R020 to BANK_SYS_TC_TR_R037
Added test cases from BANK_SYS_TC_TR_R020 to BANK_SYS_TC_TR_R037
</commit_message>
<xml_diff>
--- a/Testing/Test Cases/Transfer Page TC.xlsx
+++ b/Testing/Test Cases/Transfer Page TC.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="223">
   <si>
     <t>Project Name:</t>
   </si>
@@ -365,21 +365,6 @@
     <t>BANK_SYS_SRS_TR_R036</t>
   </si>
   <si>
-    <t>BANK_SYS_SRS_TR_R037</t>
-  </si>
-  <si>
-    <t>BANK_SYS_SRS_TR_R038</t>
-  </si>
-  <si>
-    <t>BANK_SYS_SRS_TR_R039</t>
-  </si>
-  <si>
-    <t>BANK_SYS_SRS_TR_R040</t>
-  </si>
-  <si>
-    <t>BANK_SYS_SRS_TR_R041</t>
-  </si>
-  <si>
     <t>verify that Text field account ID "  only accept numbers</t>
   </si>
   <si>
@@ -528,10 +513,286 @@
 Account ID:987654321</t>
   </si>
   <si>
-    <t>verify that customer cannot transfer money more than 10,000 for any account per transaction</t>
-  </si>
-  <si>
     <t xml:space="preserve"> error message shall be displayed  “You have exceeded the amount of money allowed to be transferred per transaction” with close icon and button with title ok </t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_TR_R043</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_TR_R044</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_TR_R045</t>
+  </si>
+  <si>
+    <t>verify that customer cannot transfer money more than 10,000LE for any account per transaction</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_TR_R011</t>
+  </si>
+  <si>
+    <t>amount : 100,000
+Account ID:987654321</t>
+  </si>
+  <si>
+    <t>verify that customer cannot transfer money more than 100,000LE for any account per transaction</t>
+  </si>
+  <si>
+    <t>amount : 100,001
+Account ID:987654321</t>
+  </si>
+  <si>
+    <t>1_enter "amount " like in test data 
+2_enter" Account ID" like in test dta
+3_press submit
+4- repeate the perevious 3 steps 10 times till the total amount of mony transferred = 100,000LE</t>
+  </si>
+  <si>
+    <t>verify that The maximum amount of money can Customer transfer to any specific current account shall be 100,000LE per day</t>
+  </si>
+  <si>
+    <t>veify that The maximum amount of money can Customer transfer to any other saving account shall be 100,000LE per transaction</t>
+  </si>
+  <si>
+    <t>verify that customer cannot transfer money more than 100,000LE  to spesific "current "  account per day</t>
+  </si>
+  <si>
+    <t>1_enter "amount " like in test data 
+2_enter" Account ID" like in test dta
+3_press submit
+4- repeate the perevious 3 steps 11 times till the total amount of mony transferred more than &gt;100,000LE</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> error message shall be displayed  “You have exceeded the amount of money allowed to be transferred per transaction” with close icon and button with title ok</t>
+  </si>
+  <si>
+    <t>1_enter "amount " like in test data 
+2_enter" Account ID" like in test dta
+3_press submit
+4- repeate the perevious 3 steps 100 times till the total amount of mony transferred = 1000,000LE</t>
+  </si>
+  <si>
+    <t>1_enter "amount " like in test data 
+2_enter" Account ID" like in test dta
+3_press submit
+4_repeat the last 3 steps 10 times</t>
+  </si>
+  <si>
+    <t>1_enter "amount " like in test data 
+2_enter" Account ID" like in test dta
+3_press submit
+4_repeat the last 3 steps 11 times and at the last repeat make the amount =50 LE</t>
+  </si>
+  <si>
+    <t>verify that The maximum amount of money can Customer transfer to any other "saving "account shall be 1000,000 per day</t>
+  </si>
+  <si>
+    <t>verify that The maximum amount of 
+verify that customer cannot transfer money more than 1000,000LE  to spesific "saving "  account per day</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_TR_R013
+BANK_SYS_SRS_TR_R014</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_TR_R012
+BANK_SYS_SRS_TR_R014</t>
+  </si>
+  <si>
+    <t>1_enter "amount " like in test data 
+2_enter" Account ID" like in test dta
+3_press submit
+4- repeate the perevious 3 steps 101 time at the last repeat make the amount = 50 LE
+total money tansfered 1000,050 LE</t>
+  </si>
+  <si>
+    <t>1_enter "amount " like in test data 
+2_enter" Account ID" like in test dta
+3_press submit
+4- repeate the perevious 3 steps 11 times at the last repeate make the amount of money -50 LE total money transferred = 100,050 LE</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_TR_R009
+BANK_SYS_SRS_TR_R016</t>
+  </si>
+  <si>
+    <t>verify that The minimum amount of money Customer can transfer is 50 L.E</t>
+  </si>
+  <si>
+    <t>amount : 49
+Account ID:987654321</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> error message shall be displayed  “You cannot transfer less than 50 LE  ” with close icon and button with title ok</t>
+  </si>
+  <si>
+    <t>verify that customer cannot transfer amount less than 50 LE</t>
+  </si>
+  <si>
+    <t>amount : 50
+Account ID:987654321</t>
+  </si>
+  <si>
+    <t>1_enter" Amount" like in test data
+2_press submit</t>
+  </si>
+  <si>
+    <t>1_press drop box with label "bank name " ensure that the default value is "ITI"</t>
+  </si>
+  <si>
+    <t>The default value of 
+the dropbox with title “bank” in 
+the transfer page is “Our bank”,"ITI"</t>
+  </si>
+  <si>
+    <t>verify that The default value of 
+the dropbox with title “bank name” in 
+the transfer page is “Our bank”,"ITI"</t>
+  </si>
+  <si>
+    <t>verify that Customer can
+ transfer money to “CIB” bank
+using account in the "CIB" bank</t>
+  </si>
+  <si>
+    <t>transfer money shall be completed and pop up window appear "Done" with close icon and button with title ok</t>
+  </si>
+  <si>
+    <t>1_enter "amount " like in test data 
+2_enter" Account ID" like in test dta
+3_choose"CIB" from "bank name" drop down menu
+3_press submit</t>
+  </si>
+  <si>
+    <t>verify that Customer can transfer to  account from type " savings "</t>
+  </si>
+  <si>
+    <t>1_enter "amount " like in test data 
+2_enter" Account ID" like in test data
+3_choose our bank"ITI" from the "bank name " drop down menu
+4_press submit</t>
+  </si>
+  <si>
+    <t>1_enter "amount " like in test data 
+2_enter" Account ID" like in test dta
+3_choose" HSBC" from the "bank name " drop down menu
+4_press submit</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_TR_R009
+BANK_SYS_SRS_TR_R016
+BANK_SYS_SRS_TR_R023</t>
+  </si>
+  <si>
+    <t>verify that Customer can
+ transfer money to “QNB” bank
+using account in the "QNB" bank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">amount : 3000
+Account ID:987654321
+</t>
+  </si>
+  <si>
+    <t>1_enter "amount " like in test data 
+2_enter" Account ID" like in test dta
+3_choose"QNB" from "bank name" drop down menu
+3_press submit</t>
+  </si>
+  <si>
+    <t>verify that Customer can
+ transfer money to “AHLI” bank
+using account in the "AHLI" bank</t>
+  </si>
+  <si>
+    <t>1_enter "amount " like in test data 
+2_enter" Account ID" like in test dta
+3_choose"AHLI" from "bank name" drop down menu
+3_press submit</t>
+  </si>
+  <si>
+    <t>1_enter "amount " like in test data 
+2_enter" Account ID" like in test dta
+3_choose"Misr" from "bank name" drop down menu
+3_press submit</t>
+  </si>
+  <si>
+    <t>verify that Customer can
+ transfer money to “Misr” bank
+using account in the "Misr" bank</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_TR_R008
+BANK_SYS_SRS_TR_R027</t>
+  </si>
+  <si>
+    <t>verify that Transfer page shall contain drop box with title bank name contains “HSBC”name with our bank as default value</t>
+  </si>
+  <si>
+    <t>1_press drop box with label "bank name " ensure that the default value is "ITI"
+2_ensure that "HSBC" is listed</t>
+  </si>
+  <si>
+    <t>verify that Transfer page shall contain drop box with title bank name contains “QNB”name with our bank as default value</t>
+  </si>
+  <si>
+    <t>1_press drop box with label "bank name " ensure that the default value is "ITI"
+2_ensure that "QNB" is listed</t>
+  </si>
+  <si>
+    <t>mediun</t>
+  </si>
+  <si>
+    <t>verify that Transfer page shall contain drop box with title bank name contains “AHLI”name with our bank as default value</t>
+  </si>
+  <si>
+    <t>1_press drop box with label "bank name " ensure that the default value is "ITI"
+2_ensure that "AHLI" is listed</t>
+  </si>
+  <si>
+    <t>The dropbox with title “bank name” in 
+the transfer page contains "AHLI"</t>
+  </si>
+  <si>
+    <t>The dropbox with title “bank name” in 
+the transfer page contains "QNB"</t>
+  </si>
+  <si>
+    <t>The dropbox with title “bank name” in 
+the transfer page contains "HSBC"</t>
+  </si>
+  <si>
+    <t>verify that Transfer page shall contain drop box with title bank name contains “MISR”name with our bank as default value</t>
+  </si>
+  <si>
+    <t>1_press drop box with label "bank name " ensure that the default value is "ITI"
+2_ensure that "MISR" is listed</t>
+  </si>
+  <si>
+    <t>The dropbox with title “bank name” in 
+the transfer page contains "MISR"</t>
+  </si>
+  <si>
+    <t>verify that Transfer page  has button with title accounts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-look at the transfer page 
+            2-ensure that button with title accounts is there </t>
+  </si>
+  <si>
+    <t>Transfer page  has button with title accounts</t>
+  </si>
+  <si>
+    <t>verify that Customer  redirected to main page if he clicks on accounts button in transfer page</t>
+  </si>
+  <si>
+    <t>1_press "accounts " button</t>
+  </si>
+  <si>
+    <t>Customer  redirected to main page if he clicks on accounts button in transfer page</t>
+  </si>
+  <si>
+    <t>functional</t>
   </si>
 </sst>
 </file>
@@ -1019,10 +1280,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L57"/>
+  <dimension ref="A1:L48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1156,7 +1417,7 @@
       </c>
       <c r="D9" s="18"/>
       <c r="E9" s="18" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="F9" s="18" t="s">
         <v>91</v>
@@ -1187,7 +1448,7 @@
         <v>94</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="G10" s="18"/>
       <c r="H10" s="18" t="s">
@@ -1266,10 +1527,10 @@
       </c>
       <c r="D13" s="18"/>
       <c r="E13" s="18" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="F13" s="18" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="G13" s="18"/>
       <c r="H13" s="18" t="s">
@@ -1288,16 +1549,16 @@
         <v>62</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="E14" s="18" t="s">
         <v>94</v>
       </c>
       <c r="F14" s="18" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="G14" s="18"/>
       <c r="H14" s="18" t="s">
@@ -1310,22 +1571,22 @@
     </row>
     <row r="15" spans="1:12" s="19" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="18" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="B15" s="17" t="s">
         <v>63</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="E15" s="18" t="s">
         <v>94</v>
       </c>
       <c r="F15" s="18" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="G15" s="18"/>
       <c r="H15" s="18" t="s">
@@ -1338,22 +1599,22 @@
     </row>
     <row r="16" spans="1:12" s="19" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="18" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="B16" s="17" t="s">
         <v>64</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>119</v>
+        <v>184</v>
       </c>
       <c r="F16" s="18" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="G16" s="18"/>
       <c r="H16" s="18" t="s">
@@ -1372,18 +1633,18 @@
         <v>65</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="D17" s="18"/>
       <c r="E17" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="F17" s="18" t="s">
         <v>132</v>
-      </c>
-      <c r="F17" s="18" t="s">
-        <v>137</v>
       </c>
       <c r="G17" s="18"/>
       <c r="H17" s="18" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="I17" s="18" t="s">
         <v>92</v>
@@ -1398,18 +1659,18 @@
         <v>66</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="D18" s="18"/>
       <c r="E18" s="18" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="F18" s="18" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="G18" s="18"/>
       <c r="H18" s="18" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="I18" s="18" t="s">
         <v>92</v>
@@ -1424,14 +1685,14 @@
         <v>67</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="D19" s="18"/>
       <c r="E19" s="18" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="F19" s="18" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="G19" s="18"/>
       <c r="H19" s="18" t="s">
@@ -1443,23 +1704,23 @@
       <c r="J19" s="18"/>
     </row>
     <row r="20" spans="1:10" s="19" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="17" t="s">
-        <v>31</v>
+      <c r="A20" s="18" t="s">
+        <v>202</v>
       </c>
       <c r="B20" s="17" t="s">
         <v>68</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="E20" s="18" t="s">
         <v>94</v>
       </c>
       <c r="F20" s="18" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="G20" s="18"/>
       <c r="H20" s="18" t="s">
@@ -1471,23 +1732,23 @@
       <c r="J20" s="18"/>
     </row>
     <row r="21" spans="1:10" s="19" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="17" t="s">
-        <v>32</v>
+      <c r="A21" s="18" t="s">
+        <v>178</v>
       </c>
       <c r="B21" s="17" t="s">
         <v>69</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="E21" s="18" t="s">
         <v>94</v>
       </c>
       <c r="F21" s="18" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="G21" s="18"/>
       <c r="H21" s="18" t="s">
@@ -1499,23 +1760,23 @@
       <c r="J21" s="18"/>
     </row>
     <row r="22" spans="1:10" s="19" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="17" t="s">
-        <v>32</v>
+      <c r="A22" s="18" t="s">
+        <v>178</v>
       </c>
       <c r="B22" s="17" t="s">
         <v>70</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>151</v>
+        <v>191</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="E22" s="18" t="s">
         <v>94</v>
       </c>
       <c r="F22" s="18" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="G22" s="18"/>
       <c r="H22" s="18" t="s">
@@ -1527,23 +1788,23 @@
       <c r="J22" s="18"/>
     </row>
     <row r="23" spans="1:10" s="19" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="17" t="s">
-        <v>32</v>
+      <c r="A23" s="18" t="s">
+        <v>178</v>
       </c>
       <c r="B23" s="17" t="s">
         <v>71</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="E23" s="18" t="s">
-        <v>94</v>
+        <v>192</v>
       </c>
       <c r="F23" s="18" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="G23" s="18"/>
       <c r="H23" s="18" t="s">
@@ -1555,23 +1816,23 @@
       <c r="J23" s="18"/>
     </row>
     <row r="24" spans="1:10" s="19" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="17" t="s">
-        <v>32</v>
+      <c r="A24" s="18" t="s">
+        <v>194</v>
       </c>
       <c r="B24" s="17" t="s">
         <v>72</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E24" s="18" t="s">
-        <v>94</v>
+        <v>193</v>
       </c>
       <c r="F24" s="18" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="G24" s="18"/>
       <c r="H24" s="18" t="s">
@@ -1584,476 +1845,592 @@
     </row>
     <row r="25" spans="1:10" s="19" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="17" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B25" s="17" t="s">
         <v>73</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D25" s="18" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E25" s="18" t="s">
         <v>94</v>
       </c>
       <c r="F25" s="18" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="G25" s="18"/>
-      <c r="H25" s="18" t="s">
-        <v>20</v>
-      </c>
+      <c r="H25" s="18"/>
       <c r="I25" s="18" t="s">
         <v>21</v>
       </c>
       <c r="J25" s="18"/>
     </row>
-    <row r="26" spans="1:10" s="19" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" s="19" customFormat="1" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="17" t="s">
         <v>33</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D26" s="18" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="E26" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="F26" s="18"/>
+      <c r="F26" s="18" t="s">
+        <v>154</v>
+      </c>
       <c r="G26" s="18"/>
-      <c r="H26" s="18"/>
+      <c r="H26" s="18" t="s">
+        <v>126</v>
+      </c>
       <c r="I26" s="18" t="s">
         <v>21</v>
       </c>
       <c r="J26" s="18"/>
     </row>
-    <row r="27" spans="1:10" s="19" customFormat="1" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" s="19" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="17" t="s">
-        <v>33</v>
+        <v>159</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="D27" s="18" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="E27" s="18" t="s">
-        <v>94</v>
+        <v>170</v>
       </c>
       <c r="F27" s="18" t="s">
-        <v>160</v>
+        <v>145</v>
       </c>
       <c r="G27" s="18"/>
       <c r="H27" s="18" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="I27" s="18" t="s">
         <v>21</v>
       </c>
       <c r="J27" s="18"/>
     </row>
-    <row r="28" spans="1:10" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" s="19" customFormat="1" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="17" t="s">
-        <v>34</v>
+        <v>159</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
+        <v>76</v>
+      </c>
+      <c r="C28" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="D28" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="E28" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="F28" s="18" t="s">
+        <v>154</v>
+      </c>
       <c r="G28" s="18"/>
-      <c r="H28" s="18"/>
-      <c r="I28" s="18"/>
+      <c r="H28" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="I28" s="18" t="s">
+        <v>21</v>
+      </c>
       <c r="J28" s="18"/>
     </row>
-    <row r="29" spans="1:10" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="17" t="s">
-        <v>35</v>
+    <row r="29" spans="1:10" s="19" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="18" t="s">
+        <v>175</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
+        <v>77</v>
+      </c>
+      <c r="C29" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="D29" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="E29" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="F29" s="18" t="s">
+        <v>145</v>
+      </c>
       <c r="G29" s="18"/>
-      <c r="H29" s="18"/>
-      <c r="I29" s="18"/>
+      <c r="H29" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="I29" s="18" t="s">
+        <v>21</v>
+      </c>
       <c r="J29" s="18"/>
     </row>
-    <row r="30" spans="1:10" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="17" t="s">
-        <v>36</v>
+    <row r="30" spans="1:10" s="19" customFormat="1" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="18" t="s">
+        <v>175</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
+        <v>78</v>
+      </c>
+      <c r="C30" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="D30" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="E30" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="F30" s="18" t="s">
+        <v>168</v>
+      </c>
       <c r="G30" s="18"/>
-      <c r="H30" s="18"/>
-      <c r="I30" s="18"/>
+      <c r="H30" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="I30" s="18" t="s">
+        <v>21</v>
+      </c>
       <c r="J30" s="18"/>
     </row>
-    <row r="31" spans="1:10" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="17" t="s">
-        <v>37</v>
+    <row r="31" spans="1:10" s="19" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="18" t="s">
+        <v>174</v>
       </c>
       <c r="B31" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
+        <v>79</v>
+      </c>
+      <c r="C31" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="D31" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="E31" s="18" t="s">
+        <v>169</v>
+      </c>
+      <c r="F31" s="18" t="s">
+        <v>145</v>
+      </c>
       <c r="G31" s="18"/>
-      <c r="H31" s="18"/>
-      <c r="I31" s="18"/>
+      <c r="H31" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="I31" s="18" t="s">
+        <v>21</v>
+      </c>
       <c r="J31" s="18"/>
     </row>
-    <row r="32" spans="1:10" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="17" t="s">
-        <v>38</v>
+    <row r="32" spans="1:10" s="19" customFormat="1" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="18" t="s">
+        <v>174</v>
       </c>
       <c r="B32" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
+        <v>80</v>
+      </c>
+      <c r="C32" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="D32" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="E32" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="F32" s="18" t="s">
+        <v>168</v>
+      </c>
       <c r="G32" s="18"/>
-      <c r="H32" s="18"/>
-      <c r="I32" s="18"/>
+      <c r="H32" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="I32" s="18" t="s">
+        <v>21</v>
+      </c>
       <c r="J32" s="18"/>
     </row>
-    <row r="33" spans="1:10" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" s="19" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="17" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
+        <v>81</v>
+      </c>
+      <c r="C33" s="18" t="s">
+        <v>182</v>
+      </c>
+      <c r="D33" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="E33" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="F33" s="18" t="s">
+        <v>181</v>
+      </c>
       <c r="G33" s="18"/>
-      <c r="H33" s="18"/>
-      <c r="I33" s="18"/>
+      <c r="H33" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="I33" s="18" t="s">
+        <v>21</v>
+      </c>
       <c r="J33" s="18"/>
     </row>
-    <row r="34" spans="1:10" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" s="19" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="17" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="H34" s="18"/>
-      <c r="I34" s="18"/>
+        <v>82</v>
+      </c>
+      <c r="C34" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="D34" s="18" t="s">
+        <v>183</v>
+      </c>
+      <c r="E34" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="F34" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="G34" s="18"/>
+      <c r="H34" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="I34" s="18" t="s">
+        <v>21</v>
+      </c>
       <c r="J34" s="18"/>
     </row>
-    <row r="35" spans="1:10" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" s="19" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="17" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
+        <v>83</v>
+      </c>
+      <c r="C35" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="D35" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="E35" s="18" t="s">
+        <v>185</v>
+      </c>
+      <c r="F35" s="18" t="s">
+        <v>186</v>
+      </c>
       <c r="G35" s="18"/>
-      <c r="H35" s="18"/>
-      <c r="I35" s="18"/>
+      <c r="H35" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="I35" s="18" t="s">
+        <v>92</v>
+      </c>
       <c r="J35" s="18"/>
     </row>
-    <row r="36" spans="1:10" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" s="19" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="17" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
+        <v>84</v>
+      </c>
+      <c r="C36" s="18" t="s">
+        <v>188</v>
+      </c>
+      <c r="D36" s="18" t="s">
+        <v>196</v>
+      </c>
+      <c r="E36" s="18" t="s">
+        <v>190</v>
+      </c>
+      <c r="F36" s="18" t="s">
+        <v>189</v>
+      </c>
       <c r="G36" s="18"/>
-      <c r="H36" s="18"/>
-      <c r="I36" s="18"/>
+      <c r="H36" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="I36" s="18" t="s">
+        <v>21</v>
+      </c>
       <c r="J36" s="18"/>
     </row>
-    <row r="37" spans="1:10" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" s="19" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="17" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>81</v>
+        <v>85</v>
+      </c>
+      <c r="C37" s="18" t="s">
+        <v>195</v>
       </c>
       <c r="D37" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
+        <v>196</v>
+      </c>
+      <c r="E37" s="18" t="s">
+        <v>197</v>
+      </c>
+      <c r="F37" s="18" t="s">
+        <v>189</v>
+      </c>
       <c r="G37" s="18"/>
-      <c r="H37" s="18"/>
-      <c r="I37" s="18"/>
+      <c r="H37" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="I37" s="18" t="s">
+        <v>21</v>
+      </c>
       <c r="J37" s="18"/>
     </row>
-    <row r="38" spans="1:10" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" s="19" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="17" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="D38" s="18"/>
-      <c r="E38" s="18"/>
-      <c r="F38" s="18"/>
+        <v>86</v>
+      </c>
+      <c r="C38" s="18" t="s">
+        <v>198</v>
+      </c>
+      <c r="D38" s="18" t="s">
+        <v>196</v>
+      </c>
+      <c r="E38" s="18" t="s">
+        <v>199</v>
+      </c>
+      <c r="F38" s="18" t="s">
+        <v>189</v>
+      </c>
       <c r="G38" s="18"/>
-      <c r="H38" s="18"/>
-      <c r="I38" s="18"/>
+      <c r="H38" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="I38" s="18" t="s">
+        <v>21</v>
+      </c>
       <c r="J38" s="18"/>
     </row>
-    <row r="39" spans="1:10" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" s="19" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="17" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B39" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="D39" s="18"/>
-      <c r="E39" s="18"/>
-      <c r="F39" s="18"/>
+        <v>87</v>
+      </c>
+      <c r="C39" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="D39" s="18" t="s">
+        <v>196</v>
+      </c>
+      <c r="E39" s="18" t="s">
+        <v>200</v>
+      </c>
+      <c r="F39" s="18" t="s">
+        <v>189</v>
+      </c>
       <c r="G39" s="18"/>
-      <c r="H39" s="18"/>
-      <c r="I39" s="18"/>
+      <c r="H39" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="I39" s="18" t="s">
+        <v>21</v>
+      </c>
       <c r="J39" s="18"/>
     </row>
-    <row r="40" spans="1:10" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" s="19" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="17" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B40" s="17" t="s">
-        <v>84</v>
+        <v>88</v>
+      </c>
+      <c r="C40" s="18" t="s">
+        <v>203</v>
       </c>
       <c r="D40" s="18"/>
-      <c r="E40" s="18"/>
-      <c r="F40" s="18"/>
+      <c r="E40" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="F40" s="18" t="s">
+        <v>212</v>
+      </c>
       <c r="G40" s="18"/>
-      <c r="H40" s="18"/>
-      <c r="I40" s="18"/>
+      <c r="H40" s="18" t="s">
+        <v>207</v>
+      </c>
+      <c r="I40" s="18" t="s">
+        <v>92</v>
+      </c>
       <c r="J40" s="18"/>
     </row>
-    <row r="41" spans="1:10" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" s="19" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="17" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B41" s="17" t="s">
-        <v>85</v>
+        <v>89</v>
+      </c>
+      <c r="C41" s="18" t="s">
+        <v>205</v>
       </c>
       <c r="D41" s="18"/>
-      <c r="E41" s="18"/>
-      <c r="F41" s="18"/>
+      <c r="E41" s="18" t="s">
+        <v>206</v>
+      </c>
+      <c r="F41" s="18" t="s">
+        <v>211</v>
+      </c>
       <c r="G41" s="18"/>
-      <c r="H41" s="18"/>
-      <c r="I41" s="18"/>
+      <c r="H41" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="I41" s="18" t="s">
+        <v>92</v>
+      </c>
       <c r="J41" s="18"/>
     </row>
-    <row r="42" spans="1:10" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" s="19" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="17" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B42" s="17" t="s">
-        <v>86</v>
+        <v>104</v>
+      </c>
+      <c r="C42" s="18" t="s">
+        <v>208</v>
       </c>
       <c r="D42" s="18"/>
-      <c r="E42" s="18"/>
-      <c r="F42" s="18"/>
+      <c r="E42" s="18" t="s">
+        <v>209</v>
+      </c>
+      <c r="F42" s="18" t="s">
+        <v>210</v>
+      </c>
       <c r="G42" s="18"/>
-      <c r="H42" s="18"/>
-      <c r="I42" s="18"/>
+      <c r="H42" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="I42" s="18" t="s">
+        <v>92</v>
+      </c>
       <c r="J42" s="18"/>
     </row>
-    <row r="43" spans="1:10" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" s="19" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="17" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B43" s="17" t="s">
-        <v>87</v>
+        <v>105</v>
+      </c>
+      <c r="C43" s="18" t="s">
+        <v>213</v>
       </c>
       <c r="D43" s="18"/>
-      <c r="E43" s="18"/>
-      <c r="F43" s="18"/>
+      <c r="E43" s="18" t="s">
+        <v>214</v>
+      </c>
+      <c r="F43" s="18" t="s">
+        <v>215</v>
+      </c>
       <c r="G43" s="18"/>
-      <c r="H43" s="18"/>
-      <c r="I43" s="18"/>
+      <c r="H43" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="I43" s="18" t="s">
+        <v>92</v>
+      </c>
       <c r="J43" s="18"/>
     </row>
-    <row r="44" spans="1:10" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" s="19" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="17" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B44" s="17" t="s">
-        <v>88</v>
+        <v>106</v>
+      </c>
+      <c r="C44" s="18" t="s">
+        <v>216</v>
       </c>
       <c r="D44" s="18"/>
-      <c r="E44" s="18"/>
-      <c r="F44" s="18"/>
+      <c r="E44" s="18" t="s">
+        <v>217</v>
+      </c>
+      <c r="F44" s="18" t="s">
+        <v>218</v>
+      </c>
       <c r="G44" s="18"/>
-      <c r="H44" s="18"/>
-      <c r="I44" s="18"/>
+      <c r="H44" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="I44" s="18" t="s">
+        <v>92</v>
+      </c>
       <c r="J44" s="18"/>
     </row>
-    <row r="45" spans="1:10" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" s="19" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="17" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B45" s="17" t="s">
-        <v>89</v>
+        <v>115</v>
+      </c>
+      <c r="C45" s="18" t="s">
+        <v>219</v>
       </c>
       <c r="D45" s="18"/>
-      <c r="E45" s="18"/>
-      <c r="F45" s="18"/>
+      <c r="E45" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="F45" s="18" t="s">
+        <v>221</v>
+      </c>
       <c r="G45" s="18"/>
-      <c r="H45" s="18"/>
-      <c r="I45" s="18"/>
+      <c r="H45" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="I45" s="18" t="s">
+        <v>222</v>
+      </c>
       <c r="J45" s="18"/>
     </row>
-    <row r="46" spans="1:10" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="B46" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="D46" s="18"/>
-      <c r="E46" s="18"/>
-      <c r="F46" s="18"/>
-      <c r="G46" s="18"/>
-      <c r="H46" s="18"/>
-      <c r="I46" s="18"/>
-      <c r="J46" s="18"/>
-    </row>
-    <row r="47" spans="1:10" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="B47" s="17" t="s">
-        <v>105</v>
-      </c>
-      <c r="D47" s="18"/>
-      <c r="E47" s="18"/>
-      <c r="F47" s="18"/>
-      <c r="G47" s="18"/>
-      <c r="H47" s="18"/>
-      <c r="I47" s="18"/>
-      <c r="J47" s="18"/>
-    </row>
-    <row r="48" spans="1:10" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="B48" s="17" t="s">
-        <v>106</v>
-      </c>
-      <c r="D48" s="18"/>
-      <c r="E48" s="18"/>
-      <c r="F48" s="18"/>
-      <c r="G48" s="18"/>
-      <c r="H48" s="18"/>
-      <c r="I48" s="18"/>
-      <c r="J48" s="18"/>
-    </row>
-    <row r="49" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="B49" s="17" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="B50" s="17" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="17" t="s">
-        <v>108</v>
-      </c>
-      <c r="B51" s="17" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="B52" s="17" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="B53" s="17" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="B54" s="17" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="17" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="17" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="17" t="s">
-        <v>114</v>
-      </c>
+    <row r="46" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="17"/>
+    </row>
+    <row r="47" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="17"/>
+    </row>
+    <row r="48" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B5:K5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
edited up on comment review
edited up on comment review
</commit_message>
<xml_diff>
--- a/Testing/Test Cases/Transfer Page TC.xlsx
+++ b/Testing/Test Cases/Transfer Page TC.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\iti\project managment\review sondos\Internet-Banking-System\Testing\Test Cases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Documents\GitHub\Internet-Banking-System\Testing\Test Cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="252">
   <si>
     <t>Project Name:</t>
   </si>
@@ -95,13 +95,7 @@
     <t xml:space="preserve">Transfer page </t>
   </si>
   <si>
-    <t>BANK_SYS_SRS_TR_R002</t>
-  </si>
-  <si>
     <t>BANK_SYS_SRS_TR_R003</t>
-  </si>
-  <si>
-    <t>BANK_SYS_SRS_TR_R004</t>
   </si>
   <si>
     <t>BANK_SYS_SRS_TR_R005</t>
@@ -285,13 +279,6 @@
     <t>verify that Transfer page  contains text field with label account ID</t>
   </si>
   <si>
-    <t>amount : 5000
-Account ID: 12345678</t>
-  </si>
-  <si>
-    <t>amount : 5000</t>
-  </si>
-  <si>
     <t>BANK_SYS_TC_TR_R037</t>
   </si>
   <si>
@@ -311,10 +298,6 @@
   </si>
   <si>
     <t>Transfer page contains field with tlabel account ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1-look at the transfer page 
-            2-ensure that drop box with label bank name </t>
   </si>
   <si>
     <t>medium</t>
@@ -349,30 +332,13 @@
     <t>verify that Text field account ID " is mandatory can not be empty and error message is shown</t>
   </si>
   <si>
-    <t>amount : 5000
-Account ID:12345678
-his balance :3000</t>
-  </si>
-  <si>
     <t xml:space="preserve">error Message displayed "you don't have the required amount , please check your balance" with close icon and button with title ok </t>
   </si>
   <si>
     <t>verify that Customer can transfer to  account from type  "current "</t>
   </si>
   <si>
-    <t>amount : 5000
-Account ID:12345678</t>
-  </si>
-  <si>
-    <t>amount : 5000
-Account ID:987654321</t>
-  </si>
-  <si>
     <t xml:space="preserve">verify that customer can transfer to any account  in other bank </t>
-  </si>
-  <si>
-    <t>amount : 5000
-Account ID:011233323445</t>
   </si>
   <si>
     <t>amount : 10,000
@@ -509,35 +475,7 @@
 BANK_SYS_SRS_TR_R027</t>
   </si>
   <si>
-    <t>verify that Transfer page shall contain drop box with title bank name contains “HSBC”name with our bank as default value</t>
-  </si>
-  <si>
-    <t>verify that Transfer page shall contain drop box with title bank name contains “QNB”name with our bank as default value</t>
-  </si>
-  <si>
     <t>mediun</t>
-  </si>
-  <si>
-    <t>verify that Transfer page shall contain drop box with title bank name contains “AHLI”name with our bank as default value</t>
-  </si>
-  <si>
-    <t>The dropbox with title “bank name” in 
-the transfer page contains "AHLI"</t>
-  </si>
-  <si>
-    <t>The dropbox with title “bank name” in 
-the transfer page contains "QNB"</t>
-  </si>
-  <si>
-    <t>The dropbox with title “bank name” in 
-the transfer page contains "HSBC"</t>
-  </si>
-  <si>
-    <t>verify that Transfer page shall contain drop box with title bank name contains “MISR”name with our bank as default value</t>
-  </si>
-  <si>
-    <t>The dropbox with title “bank name” in 
-the transfer page contains "MISR"</t>
   </si>
   <si>
     <t>verify that Transfer page  has button with title accounts</t>
@@ -604,13 +542,6 @@
 2_ensure that "MISR" is listed</t>
   </si>
   <si>
-    <t>verify that Text field “amount "   accept numbers</t>
-  </si>
-  <si>
-    <t>amount : asdfg
-Account ID: 12345678</t>
-  </si>
-  <si>
     <t>transfer money shall be completed and if user returns to his account page he will find that his balance is redued by the transferred amonut "5000"</t>
   </si>
   <si>
@@ -628,34 +559,16 @@
 BANK_SYS_SRS_Log_R012</t>
   </si>
   <si>
-    <t>Account ID: 12345678</t>
-  </si>
-  <si>
     <t>Error message shall be shown  below amount field  this field is mandatory "colored with red</t>
   </si>
   <si>
     <t xml:space="preserve">verify that Text field “amount " doesnot accept special characters </t>
   </si>
   <si>
-    <t>amount : ***$$$$$
-Account ID: 12345678</t>
-  </si>
-  <si>
-    <t>verify that Text field account ID "  numbers</t>
-  </si>
-  <si>
     <t>verify that Text field account ID "  doesnot accept letters and error message is shown</t>
   </si>
   <si>
-    <t>amount : 5000
-Account ID:Aassss</t>
-  </si>
-  <si>
     <t>Error message shall be shown  below account ID field "in valid format of data "colored with red</t>
-  </si>
-  <si>
-    <t>amount : 5000
-Account ID:$$$$*****</t>
   </si>
   <si>
     <t>BANK_SYS_SRS_TR_R002
@@ -674,25 +587,6 @@
   </si>
   <si>
     <t xml:space="preserve">verify that if Customer entered amount of money greater than his balance , error Message displayed </t>
-  </si>
-  <si>
-    <t xml:space="preserve">verify that if Customer entered amount of money smaller than his balance , error Message displayed </t>
-  </si>
-  <si>
-    <t>amount : 2000
-Account ID:12345678
-his balance :3000</t>
-  </si>
-  <si>
-    <t>transfer money shall be completed and if user returns to his account page he will find that his balance is redued by the transferred amonut "2000"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">verify that if Customer entered amount of money equal to his balance , error Message displayed </t>
-  </si>
-  <si>
-    <t>amount : 3000
-Account ID:12345678
-his balance :3000</t>
   </si>
   <si>
     <t>transfer money shall be completed and if user returns to his account page he will find that his balance is redued by the transferred amonut "3000"</t>
@@ -739,9 +633,6 @@
     <t>verify that  Customer can transfer to any specific current account =100,000LE per day</t>
   </si>
   <si>
-    <t>verify that customer cannot transfer money = 100,050LE  to spesific "current "  account per day</t>
-  </si>
-  <si>
     <t xml:space="preserve"> transfer money shall not  be completed and if user returns to his account page he will find that his balance is the same no thing changed</t>
   </si>
   <si>
@@ -752,10 +643,6 @@
   </si>
   <si>
     <t>verify that Customer can transfer to any other "saving "account 1000,000 per day</t>
-  </si>
-  <si>
-    <t>verify that The maximum amount of 
-verify that customer cannot transfer money more than 1000,050LE  to spesific "saving "  account per day</t>
   </si>
   <si>
     <t>1_enter "amount " like in test data 
@@ -788,10 +675,6 @@
     <t>Reviewed comments</t>
   </si>
   <si>
-    <t xml:space="preserve">same as : BANK_SYS_TC_TR_R002
-duplicated </t>
-  </si>
-  <si>
     <t>verify that Text field account ID "  doesnot accept special characters and error message is shown</t>
   </si>
   <si>
@@ -856,6 +739,203 @@
   <si>
     <t>1- missing test case that customer try to 
 transfer money to invalid accounts.</t>
+  </si>
+  <si>
+    <t>amount : 5000
+Account ID: 12345678
+bank name drop list : defualt</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> verify that user can 
+transfer money successfully</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_TR_R002
+BANK_SYS_SRS_TR_R004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-look at the transfer page 
+ 2-ensure that drop box with label bank name </t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_TR_R005
+BANK_SYS_SRS_TR_R021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">verify that customer cannot transfer moey to invalid account </t>
+  </si>
+  <si>
+    <t>amount : asdfg
+Account ID: 12345678
+bank name drop list : defualt</t>
+  </si>
+  <si>
+    <t>amount : ***$$$$$
+Account ID: 12345678
+bank name drop list : defualt</t>
+  </si>
+  <si>
+    <t>Account ID: 12345678
+bank name drop list : defualt</t>
+  </si>
+  <si>
+    <t>amount : 5000
+Account ID:Aassss
+bank name drop list : defualt</t>
+  </si>
+  <si>
+    <t>amount : 5000
+Account ID:$$$$*****
+bank name drop list : defualt</t>
+  </si>
+  <si>
+    <t>amount : 5000
+bank name drop list : defualt</t>
+  </si>
+  <si>
+    <t>transfer money shall be completed and if user returns to his account page he will find that his balance is redued by the transferred amonut "2999"</t>
+  </si>
+  <si>
+    <t>amount : 3001
+Account ID:12345678
+his balance :3000</t>
+  </si>
+  <si>
+    <t>amount : 5000
+Account ID:12345678
+bank name drop list : defualt
+his balance :3000</t>
+  </si>
+  <si>
+    <t>amount : 5000
+Account ID:qqqqqq
+bank name drop list : defualt
+his balance :3000</t>
+  </si>
+  <si>
+    <t>amount : 2999
+Account ID:12345678
+bank name drop list : defualt
+his balance :3000</t>
+  </si>
+  <si>
+    <t>amount : 3000
+Account ID:12345678
+bank name drop list : defualt
+his balance :3000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">verify that  Customer can transfer amount of money smaller than his balance </t>
+  </si>
+  <si>
+    <t>verify that Customercan transfer  amount of money equal to his balance</t>
+  </si>
+  <si>
+    <t>verify that  Customer cannot transfer amount of money more than his balance</t>
+  </si>
+  <si>
+    <t>amount : 5000
+Account ID:12345678
+bank name drop list : defualt</t>
+  </si>
+  <si>
+    <t>amount : 5000
+Account ID:987654321
+bank name drop list : defualt</t>
+  </si>
+  <si>
+    <t>amount : 5000
+Account ID:011233323445
+bank name drop list : HSBC</t>
+  </si>
+  <si>
+    <t>1-not missing look 
+BANK_SYS_TC_TR_R019</t>
+  </si>
+  <si>
+    <t>amount : 5000
+Account ID:011233323445
+bank name drop list : default</t>
+  </si>
+  <si>
+    <t>1_enter "amount " like in test data 
+2_enter" Account ID" like in test dta
+4_press submit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">verify that customer can not  transfer money to the same account  he transferes from </t>
+  </si>
+  <si>
+    <t>verify that customer cannot transfer money more than  100,000LE  to spesific "current "  account per day</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_TR_R012
+BANK_SYS_SRS_TR_R014
+BANK_SYS_SRS_TR_R027</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> transfer money shall not  be completed and error message displyed "You have exceeded the amount of money allowed to be transferred"</t>
+  </si>
+  <si>
+    <t>verify that The maximum amount of 
+verify that customer cannot transfer money more than 1000,000LE  to spesific "saving "  account per day</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_TR_R013
+BANK_SYS_SRS_TR_R014
+BANK_SYS_SRS_TR_R027</t>
+  </si>
+  <si>
+    <t>no notification for entering
+ amount less than 50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">comments on review comments </t>
+  </si>
+  <si>
+    <t>verify that Transfer page shall contain drop box with title bank name contains “HSBC”name with our bank as default value"IBS"</t>
+  </si>
+  <si>
+    <t>The dropbox with title “bank name” default value "IBS "
+ and  contains "HSBC"</t>
+  </si>
+  <si>
+    <t>The dropbox with title “bank name” default value "IBS "
+ and  contains "QNB"</t>
+  </si>
+  <si>
+    <t>verify that Transfer page shall contain drop box with title bank name contains “QNB”name with our bank as default value"IBS"</t>
+  </si>
+  <si>
+    <t>The dropbox with title “bank name” default value "IBS "contains "AHLI"</t>
+  </si>
+  <si>
+    <t>The dropbox with title “bank name” default value "IBS "contains "MISR"</t>
+  </si>
+  <si>
+    <t>verify that Transfer page shall contain drop box with title bank name contains “AHLI”name with our bank as default value"IBS"</t>
+  </si>
+  <si>
+    <t>verify that Transfer page shall contain drop box with title bank name contains “MISR”name with our bank as default value"IBS"</t>
+  </si>
+  <si>
+    <t>verify that Customer can log out from 
+his transfer page</t>
+  </si>
+  <si>
+    <t>1_press "log out " button</t>
+  </si>
+  <si>
+    <t>Customer  redirected to log in page with empty fields</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_TR_R045</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_TR_R046</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_TR_R047</t>
   </si>
 </sst>
 </file>
@@ -946,7 +1026,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -997,11 +1077,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1080,13 +1171,16 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1369,10 +1463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K55"/>
+  <dimension ref="A1:L57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9:B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1387,17 +1481,17 @@
     <col min="9" max="9" width="16.5703125" customWidth="1"/>
     <col min="10" max="10" width="15.5703125" customWidth="1"/>
     <col min="11" max="11" width="49.85546875" customWidth="1"/>
-    <col min="12" max="12" width="33.28515625" customWidth="1"/>
+    <col min="12" max="12" width="47" customWidth="1"/>
     <col min="13" max="13" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="C1" s="20"/>
       <c r="D1" s="20"/>
       <c r="E1" s="20"/>
       <c r="F1" s="15"/>
     </row>
-    <row r="2" spans="1:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1412,7 +1506,7 @@
       </c>
       <c r="F2" s="15"/>
     </row>
-    <row r="3" spans="1:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
@@ -1427,31 +1521,31 @@
       </c>
       <c r="F3" s="15"/>
     </row>
-    <row r="4" spans="1:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B4" s="3"/>
       <c r="C4" s="20"/>
       <c r="D4" s="27"/>
       <c r="E4" s="22"/>
       <c r="F4" s="15"/>
     </row>
-    <row r="5" spans="1:11" s="4" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B5" s="28"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="29"/>
-      <c r="J5" s="29"/>
-      <c r="K5" s="29"/>
-    </row>
-    <row r="6" spans="1:11" s="8" customFormat="1" ht="105" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" s="4" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="B5" s="29"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="30"/>
+      <c r="K5" s="30"/>
+    </row>
+    <row r="6" spans="1:12" s="8" customFormat="1" ht="105" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>158</v>
+        <v>141</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
@@ -1463,13 +1557,13 @@
       <c r="J6" s="7"/>
       <c r="K6" s="7"/>
     </row>
-    <row r="7" spans="1:11" s="9" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" s="9" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="23"/>
       <c r="D7" s="23"/>
       <c r="E7" s="23"/>
       <c r="F7" s="16"/>
     </row>
-    <row r="8" spans="1:11" s="10" customFormat="1" ht="19.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" s="10" customFormat="1" ht="19.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>7</v>
       </c>
@@ -1501,53 +1595,56 @@
         <v>16</v>
       </c>
       <c r="K8" s="10" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" s="11" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+      <c r="L8" s="10" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="11" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D9" s="24"/>
       <c r="E9" s="24" t="s">
-        <v>156</v>
+        <v>139</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G9" s="12"/>
       <c r="H9" s="12" t="s">
         <v>17</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="J9" s="12"/>
     </row>
-    <row r="10" spans="1:11" s="13" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
-        <v>23</v>
+    <row r="10" spans="1:12" s="13" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
+        <v>205</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>167</v>
+        <v>204</v>
       </c>
       <c r="D10" s="24" t="s">
-        <v>84</v>
+        <v>203</v>
       </c>
       <c r="E10" s="24" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>169</v>
+        <v>150</v>
       </c>
       <c r="G10" s="12"/>
       <c r="H10" s="12" t="s">
@@ -1557,28 +1654,28 @@
         <v>18</v>
       </c>
       <c r="J10" s="12"/>
-      <c r="K10" s="30" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" s="13" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K10" s="28" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" s="13" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>171</v>
+        <v>152</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>217</v>
+        <v>186</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>168</v>
+        <v>209</v>
       </c>
       <c r="E11" s="24" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F11" s="18" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
       <c r="G11" s="12"/>
       <c r="H11" s="12" t="s">
@@ -1589,24 +1686,24 @@
       </c>
       <c r="J11" s="12"/>
     </row>
-    <row r="12" spans="1:11" s="13" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" s="13" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>183</v>
+        <v>159</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>176</v>
+        <v>156</v>
       </c>
       <c r="D12" s="24" t="s">
-        <v>177</v>
+        <v>210</v>
       </c>
       <c r="E12" s="24" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F12" s="18" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
       <c r="G12" s="12"/>
       <c r="H12" s="12" t="s">
@@ -1617,24 +1714,24 @@
       </c>
       <c r="J12" s="12"/>
     </row>
-    <row r="13" spans="1:11" s="13" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" s="13" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="D13" s="24" t="s">
-        <v>174</v>
+        <v>211</v>
       </c>
       <c r="E13" s="24" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F13" s="18" t="s">
-        <v>175</v>
+        <v>155</v>
       </c>
       <c r="G13" s="12"/>
       <c r="H13" s="12" t="s">
@@ -1645,81 +1742,78 @@
       </c>
       <c r="J13" s="12"/>
     </row>
-    <row r="14" spans="1:11" s="13" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" s="13" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C14" s="24" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D14" s="24"/>
       <c r="E14" s="24" t="s">
-        <v>157</v>
+        <v>140</v>
       </c>
       <c r="F14" s="18" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="G14" s="12"/>
       <c r="H14" s="12" t="s">
         <v>17</v>
       </c>
       <c r="I14" s="12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="J14" s="12"/>
     </row>
-    <row r="15" spans="1:11" s="13" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
-        <v>25</v>
+    <row r="15" spans="1:12" s="13" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="12" t="s">
+        <v>160</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C15" s="24" t="s">
-        <v>178</v>
+        <v>157</v>
       </c>
       <c r="D15" s="24" t="s">
-        <v>84</v>
+        <v>212</v>
       </c>
       <c r="E15" s="24" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F15" s="18" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="G15" s="12"/>
       <c r="H15" s="12" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="I15" s="12" t="s">
         <v>18</v>
       </c>
       <c r="J15" s="12"/>
-      <c r="K15" s="30" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" s="13" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:12" s="13" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>184</v>
+        <v>160</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C16" s="24" t="s">
-        <v>179</v>
+        <v>188</v>
       </c>
       <c r="D16" s="24" t="s">
-        <v>180</v>
+        <v>213</v>
       </c>
       <c r="E16" s="24" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F16" s="18" t="s">
-        <v>181</v>
+        <v>158</v>
       </c>
       <c r="G16" s="12"/>
       <c r="H16" s="12" t="s">
@@ -1730,24 +1824,24 @@
       </c>
       <c r="J16" s="12"/>
     </row>
-    <row r="17" spans="1:11" s="13" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" s="13" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>184</v>
+        <v>161</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C17" s="24" t="s">
-        <v>220</v>
+        <v>98</v>
       </c>
       <c r="D17" s="24" t="s">
-        <v>182</v>
+        <v>214</v>
       </c>
       <c r="E17" s="24" t="s">
-        <v>77</v>
+        <v>118</v>
       </c>
       <c r="F17" s="18" t="s">
-        <v>181</v>
+        <v>162</v>
       </c>
       <c r="G17" s="12"/>
       <c r="H17" s="12" t="s">
@@ -1758,133 +1852,136 @@
       </c>
       <c r="J17" s="12"/>
     </row>
-    <row r="18" spans="1:11" s="13" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="12" t="s">
-        <v>185</v>
+    <row r="18" spans="1:12" s="13" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
+        <v>24</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C18" s="24" t="s">
-        <v>103</v>
-      </c>
-      <c r="D18" s="24" t="s">
-        <v>85</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="D18" s="24"/>
       <c r="E18" s="24" t="s">
-        <v>127</v>
+        <v>90</v>
       </c>
       <c r="F18" s="18" t="s">
-        <v>186</v>
+        <v>95</v>
       </c>
       <c r="G18" s="12"/>
       <c r="H18" s="12" t="s">
-        <v>19</v>
+        <v>89</v>
       </c>
       <c r="I18" s="12" t="s">
-        <v>18</v>
+        <v>74</v>
       </c>
       <c r="J18" s="12"/>
     </row>
-    <row r="19" spans="1:11" s="13" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="11" t="s">
-        <v>26</v>
+    <row r="19" spans="1:12" s="13" customFormat="1" ht="54.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="12" t="s">
+        <v>207</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D19" s="24"/>
       <c r="E19" s="24" t="s">
-        <v>95</v>
+        <v>206</v>
       </c>
       <c r="F19" s="18" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="G19" s="12"/>
       <c r="H19" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="I19" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="J19" s="12"/>
+      <c r="K19" s="28" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" s="13" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" s="24" t="s">
         <v>94</v>
-      </c>
-      <c r="I19" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="J19" s="12"/>
-    </row>
-    <row r="20" spans="1:11" s="13" customFormat="1" ht="54.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="C20" s="24" t="s">
-        <v>98</v>
       </c>
       <c r="D20" s="24"/>
       <c r="E20" s="24" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="F20" s="18" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G20" s="12"/>
       <c r="H20" s="12" t="s">
-        <v>94</v>
+        <v>17</v>
       </c>
       <c r="I20" s="12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="J20" s="12"/>
-      <c r="K20" s="30" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" s="13" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
-        <v>27</v>
+    </row>
+    <row r="21" spans="1:12" s="13" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="12" t="s">
+        <v>131</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C21" s="24" t="s">
+        <v>163</v>
+      </c>
+      <c r="D21" s="24" t="s">
+        <v>217</v>
+      </c>
+      <c r="E21" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="F21" s="18" t="s">
         <v>99</v>
-      </c>
-      <c r="D21" s="24"/>
-      <c r="E21" s="24" t="s">
-        <v>101</v>
-      </c>
-      <c r="F21" s="18" t="s">
-        <v>102</v>
       </c>
       <c r="G21" s="12"/>
       <c r="H21" s="12" t="s">
         <v>17</v>
       </c>
       <c r="I21" s="12" t="s">
-        <v>76</v>
+        <v>18</v>
       </c>
       <c r="J21" s="12"/>
-    </row>
-    <row r="22" spans="1:11" s="13" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K21" s="28" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" s="13" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C22" s="24" t="s">
-        <v>187</v>
+        <v>208</v>
       </c>
       <c r="D22" s="24" t="s">
-        <v>104</v>
+        <v>218</v>
       </c>
       <c r="E22" s="24" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F22" s="18" t="s">
-        <v>105</v>
+        <v>174</v>
       </c>
       <c r="G22" s="12"/>
       <c r="H22" s="12" t="s">
@@ -1894,28 +1991,26 @@
         <v>18</v>
       </c>
       <c r="J22" s="12"/>
-      <c r="K22" s="30" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" s="13" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K22" s="28"/>
+    </row>
+    <row r="23" spans="1:12" s="13" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C23" s="24" t="s">
-        <v>188</v>
+        <v>221</v>
       </c>
       <c r="D23" s="24" t="s">
-        <v>189</v>
+        <v>219</v>
       </c>
       <c r="E23" s="24" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F23" s="18" t="s">
-        <v>190</v>
+        <v>215</v>
       </c>
       <c r="G23" s="12"/>
       <c r="H23" s="12" t="s">
@@ -1925,28 +2020,28 @@
         <v>18</v>
       </c>
       <c r="J23" s="12"/>
-      <c r="K23" s="30" t="s">
+      <c r="K23" s="28" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" s="13" customFormat="1" ht="144.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" s="24" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" s="13" customFormat="1" ht="144.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="C24" s="24" t="s">
-        <v>191</v>
-      </c>
       <c r="D24" s="24" t="s">
-        <v>192</v>
+        <v>220</v>
       </c>
       <c r="E24" s="24" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F24" s="18" t="s">
-        <v>193</v>
+        <v>164</v>
       </c>
       <c r="G24" s="12"/>
       <c r="H24" s="12" t="s">
@@ -1956,28 +2051,28 @@
         <v>18</v>
       </c>
       <c r="J24" s="12"/>
-      <c r="K24" s="30" t="s">
+      <c r="K24" s="28" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" s="13" customFormat="1" ht="144.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" s="24" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" s="13" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="B25" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="C25" s="24" t="s">
-        <v>106</v>
-      </c>
       <c r="D25" s="24" t="s">
-        <v>107</v>
+        <v>216</v>
       </c>
       <c r="E25" s="24" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F25" s="18" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="G25" s="12"/>
       <c r="H25" s="12" t="s">
@@ -1987,25 +2082,28 @@
         <v>18</v>
       </c>
       <c r="J25" s="12"/>
-    </row>
-    <row r="26" spans="1:11" s="13" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K25" s="28" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" s="13" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C26" s="24" t="s">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="D26" s="24" t="s">
-        <v>108</v>
+        <v>224</v>
       </c>
       <c r="E26" s="24" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F26" s="18" t="s">
-        <v>169</v>
+        <v>150</v>
       </c>
       <c r="G26" s="12"/>
       <c r="H26" s="12" t="s">
@@ -2016,24 +2114,24 @@
       </c>
       <c r="J26" s="12"/>
     </row>
-    <row r="27" spans="1:11" s="13" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" s="13" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C27" s="24" t="s">
-        <v>194</v>
+        <v>121</v>
       </c>
       <c r="D27" s="24" t="s">
-        <v>108</v>
+        <v>225</v>
       </c>
       <c r="E27" s="24" t="s">
-        <v>159</v>
+        <v>75</v>
       </c>
       <c r="F27" s="18" t="s">
-        <v>169</v>
+        <v>150</v>
       </c>
       <c r="G27" s="12"/>
       <c r="H27" s="12" t="s">
@@ -2044,24 +2142,24 @@
       </c>
       <c r="J27" s="12"/>
     </row>
-    <row r="28" spans="1:11" s="13" customFormat="1" ht="126.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" s="13" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
-        <v>132</v>
+        <v>113</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C28" s="24" t="s">
-        <v>109</v>
+        <v>165</v>
       </c>
       <c r="D28" s="24" t="s">
-        <v>110</v>
+        <v>225</v>
       </c>
       <c r="E28" s="24" t="s">
-        <v>131</v>
+        <v>142</v>
       </c>
       <c r="F28" s="18" t="s">
-        <v>169</v>
+        <v>150</v>
       </c>
       <c r="G28" s="12"/>
       <c r="H28" s="12" t="s">
@@ -2071,371 +2169,373 @@
         <v>18</v>
       </c>
       <c r="J28" s="12"/>
-      <c r="K28" s="30" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" s="13" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="11" t="s">
-        <v>28</v>
+    </row>
+    <row r="29" spans="1:12" s="13" customFormat="1" ht="126.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="12" t="s">
+        <v>123</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C29" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="D29" s="24" t="s">
         <v>226</v>
       </c>
-      <c r="D29" s="24" t="s">
-        <v>196</v>
-      </c>
       <c r="E29" s="24" t="s">
-        <v>77</v>
+        <v>122</v>
       </c>
       <c r="F29" s="18" t="s">
-        <v>197</v>
+        <v>150</v>
       </c>
       <c r="G29" s="12"/>
       <c r="H29" s="12" t="s">
-        <v>94</v>
+        <v>17</v>
       </c>
       <c r="I29" s="12" t="s">
         <v>18</v>
       </c>
       <c r="J29" s="12"/>
-    </row>
-    <row r="30" spans="1:11" s="13" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="11" t="s">
-        <v>28</v>
+      <c r="K29" s="28" t="s">
+        <v>192</v>
+      </c>
+      <c r="L29" s="28" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" s="13" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="12" t="s">
+        <v>123</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C30" s="24" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="D30" s="24" t="s">
-        <v>111</v>
+        <v>228</v>
       </c>
       <c r="E30" s="24" t="s">
-        <v>77</v>
+        <v>229</v>
       </c>
       <c r="F30" s="18" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
       <c r="G30" s="12"/>
-      <c r="H30" s="12"/>
+      <c r="H30" s="12" t="s">
+        <v>17</v>
+      </c>
       <c r="I30" s="12" t="s">
         <v>18</v>
       </c>
       <c r="J30" s="12"/>
-    </row>
-    <row r="31" spans="1:11" s="13" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K30" s="28"/>
+      <c r="L30" s="28"/>
+    </row>
+    <row r="31" spans="1:12" s="13" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C31" s="24" t="s">
-        <v>227</v>
+        <v>194</v>
       </c>
       <c r="D31" s="24" t="s">
-        <v>112</v>
+        <v>167</v>
       </c>
       <c r="E31" s="24" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F31" s="18" t="s">
-        <v>203</v>
+        <v>168</v>
       </c>
       <c r="G31" s="12"/>
       <c r="H31" s="12" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="I31" s="12" t="s">
         <v>18</v>
       </c>
       <c r="J31" s="12"/>
     </row>
-    <row r="32" spans="1:11" s="13" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" s="13" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
-        <v>115</v>
+        <v>26</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C32" s="24" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="D32" s="24" t="s">
-        <v>202</v>
+        <v>102</v>
       </c>
       <c r="E32" s="24" t="s">
-        <v>199</v>
+        <v>75</v>
       </c>
       <c r="F32" s="18" t="s">
-        <v>200</v>
+        <v>166</v>
       </c>
       <c r="G32" s="12"/>
-      <c r="H32" s="12" t="s">
-        <v>94</v>
-      </c>
+      <c r="H32" s="12"/>
       <c r="I32" s="12" t="s">
         <v>18</v>
       </c>
       <c r="J32" s="12"/>
     </row>
-    <row r="33" spans="1:11" s="13" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" s="13" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
-        <v>115</v>
+        <v>26</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C33" s="24" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D33" s="24" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="E33" s="24" t="s">
-        <v>199</v>
+        <v>75</v>
       </c>
       <c r="F33" s="18" t="s">
-        <v>200</v>
+        <v>174</v>
       </c>
       <c r="G33" s="12"/>
       <c r="H33" s="12" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="I33" s="12" t="s">
         <v>18</v>
       </c>
       <c r="J33" s="12"/>
     </row>
-    <row r="34" spans="1:11" s="13" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" s="13" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C34" s="24" t="s">
-        <v>204</v>
+        <v>172</v>
       </c>
       <c r="D34" s="24" t="s">
-        <v>117</v>
+        <v>173</v>
       </c>
       <c r="E34" s="24" t="s">
-        <v>199</v>
+        <v>170</v>
       </c>
       <c r="F34" s="18" t="s">
-        <v>203</v>
+        <v>171</v>
       </c>
       <c r="G34" s="12"/>
       <c r="H34" s="12" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="I34" s="12" t="s">
         <v>18</v>
       </c>
       <c r="J34" s="12"/>
     </row>
-    <row r="35" spans="1:11" s="13" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="12" t="s">
-        <v>120</v>
+    <row r="35" spans="1:12" s="13" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="11" t="s">
+        <v>106</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C35" s="24" t="s">
-        <v>205</v>
+        <v>169</v>
       </c>
       <c r="D35" s="24" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E35" s="24" t="s">
-        <v>118</v>
+        <v>170</v>
       </c>
       <c r="F35" s="18" t="s">
-        <v>200</v>
+        <v>171</v>
       </c>
       <c r="G35" s="12"/>
       <c r="H35" s="12" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="I35" s="12" t="s">
         <v>18</v>
       </c>
       <c r="J35" s="12"/>
     </row>
-    <row r="36" spans="1:11" s="13" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="12" t="s">
-        <v>120</v>
+    <row r="36" spans="1:12" s="13" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="11" t="s">
+        <v>106</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C36" s="24" t="s">
-        <v>206</v>
+        <v>175</v>
       </c>
       <c r="D36" s="24" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E36" s="24" t="s">
-        <v>121</v>
+        <v>170</v>
       </c>
       <c r="F36" s="18" t="s">
-        <v>207</v>
+        <v>174</v>
       </c>
       <c r="G36" s="12"/>
       <c r="H36" s="12" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="I36" s="12" t="s">
         <v>18</v>
       </c>
       <c r="J36" s="12"/>
-      <c r="K36" s="30" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" s="13" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:12" s="13" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C37" s="24" t="s">
-        <v>209</v>
+        <v>176</v>
       </c>
       <c r="D37" s="24" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="E37" s="24" t="s">
-        <v>208</v>
+        <v>109</v>
       </c>
       <c r="F37" s="18" t="s">
-        <v>200</v>
+        <v>171</v>
       </c>
       <c r="G37" s="12"/>
       <c r="H37" s="12" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="I37" s="12" t="s">
         <v>18</v>
       </c>
       <c r="J37" s="12"/>
     </row>
-    <row r="38" spans="1:11" s="13" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" s="13" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
-        <v>119</v>
+        <v>232</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C38" s="24" t="s">
-        <v>210</v>
+        <v>231</v>
       </c>
       <c r="D38" s="24" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="E38" s="24" t="s">
-        <v>211</v>
+        <v>112</v>
       </c>
       <c r="F38" s="18" t="s">
-        <v>207</v>
+        <v>233</v>
       </c>
       <c r="G38" s="12"/>
       <c r="H38" s="12" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="I38" s="12" t="s">
         <v>18</v>
       </c>
       <c r="J38" s="12"/>
-      <c r="K38" s="30" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" s="13" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="11" t="s">
-        <v>29</v>
+      <c r="K38" s="28" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" s="13" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="12" t="s">
+        <v>110</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C39" s="24" t="s">
-        <v>125</v>
+        <v>179</v>
       </c>
       <c r="D39" s="24" t="s">
-        <v>124</v>
+        <v>107</v>
       </c>
       <c r="E39" s="24" t="s">
-        <v>77</v>
+        <v>178</v>
       </c>
       <c r="F39" s="18" t="s">
-        <v>207</v>
+        <v>171</v>
       </c>
       <c r="G39" s="12"/>
       <c r="H39" s="12" t="s">
-        <v>19</v>
+        <v>89</v>
       </c>
       <c r="I39" s="12" t="s">
         <v>18</v>
       </c>
       <c r="J39" s="12"/>
-      <c r="K39" s="30" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" s="13" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="11" t="s">
-        <v>29</v>
+    </row>
+    <row r="40" spans="1:12" s="13" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="12" t="s">
+        <v>235</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C40" s="24" t="s">
-        <v>123</v>
+        <v>234</v>
       </c>
       <c r="D40" s="24" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
       <c r="E40" s="24" t="s">
-        <v>77</v>
+        <v>180</v>
       </c>
       <c r="F40" s="18" t="s">
-        <v>214</v>
+        <v>233</v>
       </c>
       <c r="G40" s="12"/>
       <c r="H40" s="12" t="s">
-        <v>19</v>
+        <v>89</v>
       </c>
       <c r="I40" s="12" t="s">
         <v>18</v>
       </c>
       <c r="J40" s="12"/>
-    </row>
-    <row r="41" spans="1:11" s="13" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K40" s="28" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" s="13" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C41" s="24" t="s">
-        <v>212</v>
+        <v>116</v>
       </c>
       <c r="D41" s="24" t="s">
-        <v>213</v>
+        <v>115</v>
       </c>
       <c r="E41" s="24" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F41" s="18" t="s">
-        <v>215</v>
+        <v>177</v>
       </c>
       <c r="G41" s="12"/>
       <c r="H41" s="12" t="s">
@@ -2445,326 +2545,406 @@
         <v>18</v>
       </c>
       <c r="J41" s="12"/>
-    </row>
-    <row r="42" spans="1:11" s="13" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K41" s="28" t="s">
+        <v>196</v>
+      </c>
+      <c r="L41" s="28" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" s="13" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C42" s="24" t="s">
-        <v>160</v>
+        <v>114</v>
       </c>
       <c r="D42" s="24" t="s">
-        <v>20</v>
+        <v>117</v>
       </c>
       <c r="E42" s="24" t="s">
-        <v>161</v>
+        <v>75</v>
       </c>
       <c r="F42" s="18" t="s">
-        <v>162</v>
+        <v>183</v>
       </c>
       <c r="G42" s="12"/>
       <c r="H42" s="12" t="s">
         <v>19</v>
       </c>
       <c r="I42" s="12" t="s">
-        <v>76</v>
+        <v>18</v>
       </c>
       <c r="J42" s="12"/>
     </row>
-    <row r="43" spans="1:11" s="13" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" s="13" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C43" s="24" t="s">
-        <v>128</v>
+        <v>181</v>
       </c>
       <c r="D43" s="24" t="s">
-        <v>134</v>
+        <v>182</v>
       </c>
       <c r="E43" s="24" t="s">
-        <v>129</v>
+        <v>75</v>
       </c>
       <c r="F43" s="18" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="G43" s="12"/>
       <c r="H43" s="12" t="s">
-        <v>94</v>
+        <v>19</v>
       </c>
       <c r="I43" s="12" t="s">
         <v>18</v>
       </c>
       <c r="J43" s="12"/>
     </row>
-    <row r="44" spans="1:11" s="13" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" s="13" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="11" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C44" s="24" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="D44" s="24" t="s">
-        <v>134</v>
+        <v>20</v>
       </c>
       <c r="E44" s="24" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="F44" s="18" t="s">
-        <v>193</v>
+        <v>145</v>
       </c>
       <c r="G44" s="12"/>
       <c r="H44" s="12" t="s">
-        <v>94</v>
+        <v>19</v>
       </c>
       <c r="I44" s="12" t="s">
-        <v>18</v>
+        <v>74</v>
       </c>
       <c r="J44" s="12"/>
     </row>
-    <row r="45" spans="1:11" s="13" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" s="13" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="11" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C45" s="24" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
       <c r="D45" s="24" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="E45" s="24" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
       <c r="F45" s="18" t="s">
-        <v>193</v>
+        <v>164</v>
       </c>
       <c r="G45" s="12"/>
       <c r="H45" s="12" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="I45" s="12" t="s">
         <v>18</v>
       </c>
       <c r="J45" s="12"/>
     </row>
-    <row r="46" spans="1:11" s="13" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" s="13" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="11" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C46" s="24" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="D46" s="24" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="E46" s="24" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="F46" s="18" t="s">
-        <v>193</v>
+        <v>164</v>
       </c>
       <c r="G46" s="12"/>
       <c r="H46" s="12" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="I46" s="12" t="s">
         <v>18</v>
       </c>
       <c r="J46" s="12"/>
     </row>
-    <row r="47" spans="1:11" s="13" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" s="13" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="11" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C47" s="24" t="s">
-        <v>141</v>
-      </c>
-      <c r="D47" s="24"/>
+        <v>127</v>
+      </c>
+      <c r="D47" s="24" t="s">
+        <v>125</v>
+      </c>
       <c r="E47" s="24" t="s">
-        <v>163</v>
+        <v>128</v>
       </c>
       <c r="F47" s="18" t="s">
-        <v>147</v>
+        <v>164</v>
       </c>
       <c r="G47" s="12"/>
       <c r="H47" s="12" t="s">
-        <v>143</v>
+        <v>89</v>
       </c>
       <c r="I47" s="12" t="s">
-        <v>76</v>
+        <v>18</v>
       </c>
       <c r="J47" s="12"/>
-      <c r="K47" s="30" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" s="13" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:12" s="13" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="11" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C48" s="24" t="s">
-        <v>142</v>
-      </c>
-      <c r="D48" s="24"/>
+        <v>130</v>
+      </c>
+      <c r="D48" s="24" t="s">
+        <v>125</v>
+      </c>
       <c r="E48" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="F48" s="18" t="s">
         <v>164</v>
-      </c>
-      <c r="F48" s="18" t="s">
-        <v>146</v>
       </c>
       <c r="G48" s="12"/>
       <c r="H48" s="12" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="I48" s="12" t="s">
-        <v>76</v>
+        <v>18</v>
       </c>
       <c r="J48" s="12"/>
-      <c r="K48" s="30" t="s">
-        <v>229</v>
-      </c>
     </row>
     <row r="49" spans="1:11" s="13" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="11" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C49" s="24" t="s">
-        <v>144</v>
+        <v>238</v>
       </c>
       <c r="D49" s="24"/>
       <c r="E49" s="24" t="s">
-        <v>165</v>
+        <v>146</v>
       </c>
       <c r="F49" s="18" t="s">
-        <v>145</v>
+        <v>239</v>
       </c>
       <c r="G49" s="12"/>
       <c r="H49" s="12" t="s">
-        <v>94</v>
+        <v>132</v>
       </c>
       <c r="I49" s="12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="J49" s="12"/>
-      <c r="K49" s="30" t="s">
-        <v>229</v>
+      <c r="K49" s="28" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="50" spans="1:11" s="13" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="11" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C50" s="24" t="s">
-        <v>148</v>
+        <v>241</v>
       </c>
       <c r="D50" s="24"/>
       <c r="E50" s="24" t="s">
-        <v>166</v>
+        <v>147</v>
       </c>
       <c r="F50" s="18" t="s">
-        <v>149</v>
+        <v>240</v>
       </c>
       <c r="G50" s="12"/>
       <c r="H50" s="12" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="I50" s="12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="J50" s="12"/>
-      <c r="K50" s="30" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" s="13" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K50" s="28" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" s="13" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="11" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B51" s="11" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="C51" s="24" t="s">
-        <v>150</v>
+        <v>244</v>
       </c>
       <c r="D51" s="24"/>
       <c r="E51" s="24" t="s">
-        <v>216</v>
+        <v>148</v>
       </c>
       <c r="F51" s="18" t="s">
-        <v>151</v>
+        <v>242</v>
       </c>
       <c r="G51" s="12"/>
       <c r="H51" s="12" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="I51" s="12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="J51" s="12"/>
-    </row>
-    <row r="52" spans="1:11" s="13" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K51" s="28" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" s="13" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A52" s="11" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B52" s="11" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="C52" s="24" t="s">
-        <v>152</v>
+        <v>245</v>
       </c>
       <c r="D52" s="24"/>
       <c r="E52" s="24" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="F52" s="18" t="s">
-        <v>154</v>
+        <v>243</v>
       </c>
       <c r="G52" s="12"/>
       <c r="H52" s="12" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="I52" s="12" t="s">
-        <v>155</v>
+        <v>74</v>
       </c>
       <c r="J52" s="12"/>
-      <c r="K52" s="30" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="11"/>
-    </row>
-    <row r="54" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="11"/>
-    </row>
-    <row r="55" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K52" s="28" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" s="13" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B53" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="C53" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="D53" s="24"/>
+      <c r="E53" s="24" t="s">
+        <v>185</v>
+      </c>
+      <c r="F53" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="G53" s="12"/>
+      <c r="H53" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="I53" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="J53" s="12"/>
+    </row>
+    <row r="54" spans="1:11" s="13" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B54" s="11" t="s">
+        <v>250</v>
+      </c>
+      <c r="C54" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="D54" s="24"/>
+      <c r="E54" s="24" t="s">
+        <v>136</v>
+      </c>
+      <c r="F54" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="G54" s="12"/>
+      <c r="H54" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="I54" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="J54" s="12"/>
+      <c r="K54" s="28" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" ht="31.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="11"/>
+      <c r="B55" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="C55" s="24" t="s">
+        <v>246</v>
+      </c>
+      <c r="E55" s="24" t="s">
+        <v>247</v>
+      </c>
+      <c r="F55" s="18" t="s">
+        <v>248</v>
+      </c>
+      <c r="H55" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="I55" s="31" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="11"/>
+    </row>
+    <row r="57" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>